<commit_message>
FFprobe package is added  1. ffprobe is taking streams json file
</commit_message>
<xml_diff>
--- a/http_url.xlsx
+++ b/http_url.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Streams</t>
   </si>
   <si>
-    <t xml:space="preserve">http://0.0.0.0:5502</t>
+    <t xml:space="preserve">http://10.10.11.52:5502</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -143,7 +143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -155,6 +155,9 @@
       <c r="A4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://10.10.11.52:5502"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Stream to play multiple streams and generate multiple streams code added.
</commit_message>
<xml_diff>
--- a/http_url.xlsx
+++ b/http_url.xlsx
@@ -20,12 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Streams</t>
   </si>
   <si>
-    <t xml:space="preserve">http://10.10.11.52:5502</t>
+    <t xml:space="preserve">http://10.10.11.52:5501/stream1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://10.10.11.52:5502/stream2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://10.10.11.52:5503/stream3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://10.10.11.52:5504/stream4</t>
   </si>
 </sst>
 </file>
@@ -127,15 +136,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -148,15 +157,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://10.10.11.52:5502"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://10.10.11.52:5501/stream1"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://10.10.11.52:5502/"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://10.10.11.52:5503/"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://10.10.11.52:5504/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>